<commit_message>
palindromo de orden k mt determinista 4 cintas funciona
</commit_message>
<xml_diff>
--- a/Maquinas de Turing/Calculadora de diferencias.xlsx
+++ b/Maquinas de Turing/Calculadora de diferencias.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\4º INFADE\Segundo cuatrimestre\Teoria Avanzada de la Computacion\Repositorio\Maquinas de Turing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610659FA-2589-41A6-8318-28ACE7ACA940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D452F7B-6164-4B66-B46E-C341163B15A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21195" yWindow="6540" windowWidth="14805" windowHeight="11400" xr2:uid="{B0A893AB-E865-4F23-BB41-C966290884E4}"/>
+    <workbookView xWindow="11595" yWindow="4020" windowWidth="14805" windowHeight="11400" activeTab="1" xr2:uid="{B0A893AB-E865-4F23-BB41-C966290884E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -151,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -160,6 +161,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -476,16 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C17DBC7-C842-476D-8B31-523D620B37C4}">
-  <dimension ref="B3:K11"/>
+  <dimension ref="B3:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +520,9 @@
       <c r="K4" s="3">
         <v>12297</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -554,7 +559,7 @@
         <v>6657</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -587,7 +592,7 @@
         <v>3584</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -616,7 +621,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -641,7 +646,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -662,7 +667,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -679,7 +684,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -696,4 +701,135 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CA8DF3-7144-4610-A3C7-31D7ED19C5E0}">
+  <dimension ref="B1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>2*C1+2^B2-B2+3</f>
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <f>2^(B2-1)*(B11+B2+4) + B2-2</f>
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <f>B2+2^(B2-2)*(2*B2+13)-2</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>2*C2+2^B3-B3+3</f>
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <f>2^(B3-1)*(B11+B3+4) + B3-2</f>
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="0">B3+2^(B3-2)*(2*B3+13)-2</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="1">2*C3+2^B4-B4+3</f>
+        <v>99</v>
+      </c>
+      <c r="E4">
+        <f>2^(B4-1)*(B11+B4+4) + B4-2</f>
+        <v>86</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>517</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>1158</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>869</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2567</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>